<commit_message>
First pass at handling OR cases (which are really OPT).  In process.
</commit_message>
<xml_diff>
--- a/FMM_Descriptions_14Nov18.xlsx
+++ b/FMM_Descriptions_14Nov18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\dev\Projects\PCC_Utils\FMM Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\dev\Projects\convert_fmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4E2870AC-ED96-441D-94A7-8408F0BE8C9D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AFAB13-1E63-4F67-9D76-1D4006501839}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMM_Descriptions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="1350">
   <si>
     <t>Installation</t>
   </si>
@@ -4068,13 +4068,47 @@
   </si>
   <si>
     <t>enclosureType</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>airCooled</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rtdRateLimFilteredSel</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4209,8 +4243,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4396,6 +4453,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -4573,9 +4642,15 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="1" fillId="33" borderId="10" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4617,7 +4692,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="p::v Condition Cells" xfId="42"/>
+    <cellStyle name="p::v Condition Cells" xfId="42" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -4931,17 +5006,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I557"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5388,28 +5465,28 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
+      <c r="E18" s="2" t="s">
+        <v>1349</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5518,28 +5595,28 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
+      <c r="E23" s="2" t="s">
+        <v>1349</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
         <v>1</v>
       </c>
     </row>
@@ -5735,11 +5812,11 @@
       <c r="C31" t="s">
         <v>87</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E31" t="s">
-        <v>64</v>
+      <c r="E31" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
@@ -5752,28 +5829,28 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32">
+      <c r="F32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="6">
+        <v>1</v>
+      </c>
+      <c r="H32" s="6">
         <v>1</v>
       </c>
     </row>
@@ -19429,11 +19506,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">

</xml_diff>